<commit_message>
updating README and completing notebook
</commit_message>
<xml_diff>
--- a/baseline-lcia/baseline_lcia.xlsx
+++ b/baseline-lcia/baseline_lcia.xlsx
@@ -114,7 +114,7 @@
     <t>Heat-HTC</t>
   </si>
   <si>
-    <t>'Carbon dioxide, non-fossil, resource correction' (kg, None, None)</t>
+    <t>'Carbon dioxide, non-fossil, resource correction' (kilogram, None, ('natural resource', 'in air'))</t>
   </si>
   <si>
     <t>CO2 - HTC</t>
@@ -532,7 +532,7 @@
         <v>2.31E-07</v>
       </c>
       <c r="H4">
-        <v>7.37E-05</v>
+        <v>1.03E-06</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -558,7 +558,7 @@
         <v>7.58E-06</v>
       </c>
       <c r="H5">
-        <v>0.004</v>
+        <v>5.59E-05</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -584,7 +584,7 @@
         <v>1.62E-07</v>
       </c>
       <c r="H6">
-        <v>3.81E-05</v>
+        <v>5.33E-07</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -610,7 +610,7 @@
         <v>6.69E-05</v>
       </c>
       <c r="H7">
-        <v>0.0143</v>
+        <v>0.000199</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -636,7 +636,7 @@
         <v>0.000357</v>
       </c>
       <c r="H8">
-        <v>0.00554</v>
+        <v>7.75E-05</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -662,7 +662,7 @@
         <v>2.79E-06</v>
       </c>
       <c r="H9">
-        <v>8.11E-06</v>
+        <v>1.13E-07</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -688,7 +688,7 @@
         <v>6.85E-13</v>
       </c>
       <c r="H10">
-        <v>4.85E-11</v>
+        <v>6.79E-13</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -714,7 +714,7 @@
         <v>2.74E-10</v>
       </c>
       <c r="H11">
-        <v>1.22E-09</v>
+        <v>1.7E-11</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -740,7 +740,7 @@
         <v>2.57E-13</v>
       </c>
       <c r="H12">
-        <v>1.01E-10</v>
+        <v>1.42E-12</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -766,7 +766,7 @@
         <v>3.48E-08</v>
       </c>
       <c r="H13">
-        <v>2.22E-05</v>
+        <v>3.11E-07</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -792,7 +792,7 @@
         <v>2.36E-06</v>
       </c>
       <c r="H14">
-        <v>0.000427</v>
+        <v>5.97E-06</v>
       </c>
     </row>
   </sheetData>
@@ -876,7 +876,7 @@
         <v>2.27E-08</v>
       </c>
       <c r="H4">
-        <v>7.37E-05</v>
+        <v>1.03E-06</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -902,7 +902,7 @@
         <v>7.45E-07</v>
       </c>
       <c r="H5">
-        <v>0.004</v>
+        <v>5.59E-05</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -928,7 +928,7 @@
         <v>1.59E-08</v>
       </c>
       <c r="H6">
-        <v>3.81E-05</v>
+        <v>5.33E-07</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -954,7 +954,7 @@
         <v>6.58E-06</v>
       </c>
       <c r="H7">
-        <v>0.0143</v>
+        <v>0.000199</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -980,7 +980,7 @@
         <v>3.51E-05</v>
       </c>
       <c r="H8">
-        <v>0.00554</v>
+        <v>7.75E-05</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1006,7 +1006,7 @@
         <v>2.75E-07</v>
       </c>
       <c r="H9">
-        <v>8.11E-06</v>
+        <v>1.13E-07</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1032,7 +1032,7 @@
         <v>6.74E-14</v>
       </c>
       <c r="H10">
-        <v>4.85E-11</v>
+        <v>6.79E-13</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1058,7 +1058,7 @@
         <v>2.7E-11</v>
       </c>
       <c r="H11">
-        <v>1.22E-09</v>
+        <v>1.7E-11</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1084,7 +1084,7 @@
         <v>2.53E-14</v>
       </c>
       <c r="H12">
-        <v>1.01E-10</v>
+        <v>1.42E-12</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1110,7 +1110,7 @@
         <v>3.42E-09</v>
       </c>
       <c r="H13">
-        <v>2.22E-05</v>
+        <v>3.11E-07</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1136,7 +1136,7 @@
         <v>2.32E-07</v>
       </c>
       <c r="H14">
-        <v>0.000427</v>
+        <v>5.97E-06</v>
       </c>
     </row>
   </sheetData>
@@ -1220,7 +1220,7 @@
         <v>2.49E-08</v>
       </c>
       <c r="H4">
-        <v>7.37E-05</v>
+        <v>1.03E-06</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1246,7 +1246,7 @@
         <v>8.16E-07</v>
       </c>
       <c r="H5">
-        <v>0.004</v>
+        <v>5.59E-05</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1272,7 +1272,7 @@
         <v>1.74E-08</v>
       </c>
       <c r="H6">
-        <v>3.81E-05</v>
+        <v>5.33E-07</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1298,7 +1298,7 @@
         <v>7.2E-06</v>
       </c>
       <c r="H7">
-        <v>0.0143</v>
+        <v>0.000199</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1324,7 +1324,7 @@
         <v>3.85E-05</v>
       </c>
       <c r="H8">
-        <v>0.00554</v>
+        <v>7.75E-05</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1350,7 +1350,7 @@
         <v>3.01E-07</v>
       </c>
       <c r="H9">
-        <v>8.11E-06</v>
+        <v>1.13E-07</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1376,7 +1376,7 @@
         <v>7.37E-14</v>
       </c>
       <c r="H10">
-        <v>4.85E-11</v>
+        <v>6.79E-13</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1402,7 +1402,7 @@
         <v>2.95E-11</v>
       </c>
       <c r="H11">
-        <v>1.22E-09</v>
+        <v>1.7E-11</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1428,7 +1428,7 @@
         <v>2.76E-14</v>
       </c>
       <c r="H12">
-        <v>1.01E-10</v>
+        <v>1.42E-12</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1454,7 +1454,7 @@
         <v>3.74E-09</v>
       </c>
       <c r="H13">
-        <v>2.22E-05</v>
+        <v>3.11E-07</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1480,7 +1480,7 @@
         <v>2.54E-07</v>
       </c>
       <c r="H14">
-        <v>0.000427</v>
+        <v>5.97E-06</v>
       </c>
     </row>
   </sheetData>
@@ -1564,7 +1564,7 @@
         <v>2.35E-08</v>
       </c>
       <c r="H4">
-        <v>7.37E-05</v>
+        <v>1.03E-06</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1590,7 +1590,7 @@
         <v>7.69E-07</v>
       </c>
       <c r="H5">
-        <v>0.004</v>
+        <v>5.59E-05</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1616,7 +1616,7 @@
         <v>1.64E-08</v>
       </c>
       <c r="H6">
-        <v>3.81E-05</v>
+        <v>5.33E-07</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1642,7 +1642,7 @@
         <v>6.79E-06</v>
       </c>
       <c r="H7">
-        <v>0.0143</v>
+        <v>0.000199</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1668,7 +1668,7 @@
         <v>3.63E-05</v>
       </c>
       <c r="H8">
-        <v>0.00554</v>
+        <v>7.75E-05</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1694,7 +1694,7 @@
         <v>2.83E-07</v>
       </c>
       <c r="H9">
-        <v>8.11E-06</v>
+        <v>1.13E-07</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1720,7 +1720,7 @@
         <v>6.949999999999999E-14</v>
       </c>
       <c r="H10">
-        <v>4.85E-11</v>
+        <v>6.79E-13</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1746,7 +1746,7 @@
         <v>2.78E-11</v>
       </c>
       <c r="H11">
-        <v>1.22E-09</v>
+        <v>1.7E-11</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1772,7 +1772,7 @@
         <v>2.61E-14</v>
       </c>
       <c r="H12">
-        <v>1.01E-10</v>
+        <v>1.42E-12</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1798,7 +1798,7 @@
         <v>3.53E-09</v>
       </c>
       <c r="H13">
-        <v>2.22E-05</v>
+        <v>3.11E-07</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1824,7 +1824,7 @@
         <v>2.4E-07</v>
       </c>
       <c r="H14">
-        <v>0.000427</v>
+        <v>5.97E-06</v>
       </c>
     </row>
   </sheetData>
@@ -1908,7 +1908,7 @@
         <v>1.36E-08</v>
       </c>
       <c r="H4">
-        <v>7.37E-05</v>
+        <v>1.03E-06</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1934,7 +1934,7 @@
         <v>4.45E-07</v>
       </c>
       <c r="H5">
-        <v>0.004</v>
+        <v>5.59E-05</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1960,7 +1960,7 @@
         <v>9.489999999999999E-09</v>
       </c>
       <c r="H6">
-        <v>3.81E-05</v>
+        <v>5.33E-07</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1986,7 +1986,7 @@
         <v>3.92E-06</v>
       </c>
       <c r="H7">
-        <v>0.0143</v>
+        <v>0.000199</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2012,7 +2012,7 @@
         <v>2.1E-05</v>
       </c>
       <c r="H8">
-        <v>0.00554</v>
+        <v>7.75E-05</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -2038,7 +2038,7 @@
         <v>1.64E-07</v>
       </c>
       <c r="H9">
-        <v>8.11E-06</v>
+        <v>1.13E-07</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2064,7 +2064,7 @@
         <v>4.02E-14</v>
       </c>
       <c r="H10">
-        <v>4.85E-11</v>
+        <v>6.79E-13</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -2090,7 +2090,7 @@
         <v>1.61E-11</v>
       </c>
       <c r="H11">
-        <v>1.22E-09</v>
+        <v>1.7E-11</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2116,7 +2116,7 @@
         <v>1.51E-14</v>
       </c>
       <c r="H12">
-        <v>1.01E-10</v>
+        <v>1.42E-12</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2142,7 +2142,7 @@
         <v>2.04E-09</v>
       </c>
       <c r="H13">
-        <v>2.22E-05</v>
+        <v>3.11E-07</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -2168,7 +2168,7 @@
         <v>1.39E-07</v>
       </c>
       <c r="H14">
-        <v>0.000427</v>
+        <v>5.97E-06</v>
       </c>
     </row>
   </sheetData>
@@ -2252,7 +2252,7 @@
         <v>1.17E-08</v>
       </c>
       <c r="H4">
-        <v>7.37E-05</v>
+        <v>1.03E-06</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2278,7 +2278,7 @@
         <v>3.83E-07</v>
       </c>
       <c r="H5">
-        <v>0.004</v>
+        <v>5.59E-05</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2304,7 +2304,7 @@
         <v>8.17E-09</v>
       </c>
       <c r="H6">
-        <v>3.81E-05</v>
+        <v>5.33E-07</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2330,7 +2330,7 @@
         <v>3.38E-06</v>
       </c>
       <c r="H7">
-        <v>0.0143</v>
+        <v>0.000199</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2356,7 +2356,7 @@
         <v>1.8E-05</v>
       </c>
       <c r="H8">
-        <v>0.00554</v>
+        <v>7.75E-05</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -2382,7 +2382,7 @@
         <v>1.41E-07</v>
       </c>
       <c r="H9">
-        <v>8.11E-06</v>
+        <v>1.13E-07</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2408,7 +2408,7 @@
         <v>3.46E-14</v>
       </c>
       <c r="H10">
-        <v>4.85E-11</v>
+        <v>6.79E-13</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -2434,7 +2434,7 @@
         <v>1.38E-11</v>
       </c>
       <c r="H11">
-        <v>1.22E-09</v>
+        <v>1.7E-11</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2460,7 +2460,7 @@
         <v>1.3E-14</v>
       </c>
       <c r="H12">
-        <v>1.01E-10</v>
+        <v>1.42E-12</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2486,7 +2486,7 @@
         <v>1.76E-09</v>
       </c>
       <c r="H13">
-        <v>2.22E-05</v>
+        <v>3.11E-07</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -2512,7 +2512,7 @@
         <v>1.19E-07</v>
       </c>
       <c r="H14">
-        <v>0.000427</v>
+        <v>5.97E-06</v>
       </c>
     </row>
   </sheetData>
@@ -2596,7 +2596,7 @@
         <v>1.1E-08</v>
       </c>
       <c r="H4">
-        <v>7.37E-05</v>
+        <v>1.03E-06</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2622,7 +2622,7 @@
         <v>3.61E-07</v>
       </c>
       <c r="H5">
-        <v>0.004</v>
+        <v>5.59E-05</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2648,7 +2648,7 @@
         <v>7.699999999999999E-09</v>
       </c>
       <c r="H6">
-        <v>3.81E-05</v>
+        <v>5.33E-07</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2674,7 +2674,7 @@
         <v>3.18E-06</v>
       </c>
       <c r="H7">
-        <v>0.0143</v>
+        <v>0.000199</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2700,7 +2700,7 @@
         <v>1.7E-05</v>
       </c>
       <c r="H8">
-        <v>0.00554</v>
+        <v>7.75E-05</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -2726,7 +2726,7 @@
         <v>1.33E-07</v>
       </c>
       <c r="H9">
-        <v>8.11E-06</v>
+        <v>1.13E-07</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2752,7 +2752,7 @@
         <v>3.26E-14</v>
       </c>
       <c r="H10">
-        <v>4.85E-11</v>
+        <v>6.79E-13</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -2778,7 +2778,7 @@
         <v>1.3E-11</v>
       </c>
       <c r="H11">
-        <v>1.22E-09</v>
+        <v>1.7E-11</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2804,7 +2804,7 @@
         <v>1.22E-14</v>
       </c>
       <c r="H12">
-        <v>1.01E-10</v>
+        <v>1.42E-12</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2830,7 +2830,7 @@
         <v>1.65E-09</v>
       </c>
       <c r="H13">
-        <v>2.22E-05</v>
+        <v>3.11E-07</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -2856,7 +2856,7 @@
         <v>1.12E-07</v>
       </c>
       <c r="H14">
-        <v>0.000427</v>
+        <v>5.97E-06</v>
       </c>
     </row>
   </sheetData>
@@ -2940,7 +2940,7 @@
         <v>1.05E-08</v>
       </c>
       <c r="H4">
-        <v>7.37E-05</v>
+        <v>1.03E-06</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2966,7 +2966,7 @@
         <v>3.45E-07</v>
       </c>
       <c r="H5">
-        <v>0.004</v>
+        <v>5.59E-05</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2992,7 +2992,7 @@
         <v>7.37E-09</v>
       </c>
       <c r="H6">
-        <v>3.81E-05</v>
+        <v>5.33E-07</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -3018,7 +3018,7 @@
         <v>3.04E-06</v>
       </c>
       <c r="H7">
-        <v>0.0143</v>
+        <v>0.000199</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -3044,7 +3044,7 @@
         <v>1.63E-05</v>
       </c>
       <c r="H8">
-        <v>0.00554</v>
+        <v>7.75E-05</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -3070,7 +3070,7 @@
         <v>1.27E-07</v>
       </c>
       <c r="H9">
-        <v>8.11E-06</v>
+        <v>1.13E-07</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -3096,7 +3096,7 @@
         <v>3.12E-14</v>
       </c>
       <c r="H10">
-        <v>4.85E-11</v>
+        <v>6.79E-13</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -3122,7 +3122,7 @@
         <v>1.25E-11</v>
       </c>
       <c r="H11">
-        <v>1.22E-09</v>
+        <v>1.7E-11</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -3148,7 +3148,7 @@
         <v>1.17E-14</v>
       </c>
       <c r="H12">
-        <v>1.01E-10</v>
+        <v>1.42E-12</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -3174,7 +3174,7 @@
         <v>1.58E-09</v>
       </c>
       <c r="H13">
-        <v>2.22E-05</v>
+        <v>3.11E-07</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -3200,7 +3200,7 @@
         <v>1.08E-07</v>
       </c>
       <c r="H14">
-        <v>0.000427</v>
+        <v>5.97E-06</v>
       </c>
     </row>
   </sheetData>
@@ -3284,7 +3284,7 @@
         <v>1.11E-08</v>
       </c>
       <c r="H4">
-        <v>7.37E-05</v>
+        <v>1.03E-06</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -3310,7 +3310,7 @@
         <v>3.66E-07</v>
       </c>
       <c r="H5">
-        <v>0.004</v>
+        <v>5.59E-05</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -3336,7 +3336,7 @@
         <v>7.8E-09</v>
       </c>
       <c r="H6">
-        <v>3.81E-05</v>
+        <v>5.33E-07</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -3362,7 +3362,7 @@
         <v>3.22E-06</v>
       </c>
       <c r="H7">
-        <v>0.0143</v>
+        <v>0.000199</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -3388,7 +3388,7 @@
         <v>1.72E-05</v>
       </c>
       <c r="H8">
-        <v>0.00554</v>
+        <v>7.75E-05</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -3414,7 +3414,7 @@
         <v>1.35E-07</v>
       </c>
       <c r="H9">
-        <v>8.11E-06</v>
+        <v>1.13E-07</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -3440,7 +3440,7 @@
         <v>3.3E-14</v>
       </c>
       <c r="H10">
-        <v>4.85E-11</v>
+        <v>6.79E-13</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -3466,7 +3466,7 @@
         <v>1.32E-11</v>
       </c>
       <c r="H11">
-        <v>1.22E-09</v>
+        <v>1.7E-11</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -3492,7 +3492,7 @@
         <v>1.24E-14</v>
       </c>
       <c r="H12">
-        <v>1.01E-10</v>
+        <v>1.42E-12</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -3518,7 +3518,7 @@
         <v>1.68E-09</v>
       </c>
       <c r="H13">
-        <v>2.22E-05</v>
+        <v>3.11E-07</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -3544,7 +3544,7 @@
         <v>1.14E-07</v>
       </c>
       <c r="H14">
-        <v>0.000427</v>
+        <v>5.97E-06</v>
       </c>
     </row>
   </sheetData>
@@ -3628,7 +3628,7 @@
         <v>1.03E-08</v>
       </c>
       <c r="H4">
-        <v>7.37E-05</v>
+        <v>1.03E-06</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -3654,7 +3654,7 @@
         <v>3.37E-07</v>
       </c>
       <c r="H5">
-        <v>0.004</v>
+        <v>5.59E-05</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -3680,7 +3680,7 @@
         <v>7.19E-09</v>
       </c>
       <c r="H6">
-        <v>3.81E-05</v>
+        <v>5.33E-07</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -3706,7 +3706,7 @@
         <v>2.97E-06</v>
       </c>
       <c r="H7">
-        <v>0.0143</v>
+        <v>0.000199</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -3732,7 +3732,7 @@
         <v>1.59E-05</v>
       </c>
       <c r="H8">
-        <v>0.00554</v>
+        <v>7.75E-05</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -3758,7 +3758,7 @@
         <v>1.24E-07</v>
       </c>
       <c r="H9">
-        <v>8.11E-06</v>
+        <v>1.13E-07</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -3784,7 +3784,7 @@
         <v>3.05E-14</v>
       </c>
       <c r="H10">
-        <v>4.85E-11</v>
+        <v>6.79E-13</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -3810,7 +3810,7 @@
         <v>1.22E-11</v>
       </c>
       <c r="H11">
-        <v>1.22E-09</v>
+        <v>1.7E-11</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -3836,7 +3836,7 @@
         <v>1.14E-14</v>
       </c>
       <c r="H12">
-        <v>1.01E-10</v>
+        <v>1.42E-12</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -3862,7 +3862,7 @@
         <v>1.55E-09</v>
       </c>
       <c r="H13">
-        <v>2.22E-05</v>
+        <v>3.11E-07</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -3888,7 +3888,7 @@
         <v>1.05E-07</v>
       </c>
       <c r="H14">
-        <v>0.000427</v>
+        <v>5.97E-06</v>
       </c>
     </row>
   </sheetData>
@@ -3972,7 +3972,7 @@
         <v>1.51E-07</v>
       </c>
       <c r="H4">
-        <v>7.37E-05</v>
+        <v>1.03E-06</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -3998,7 +3998,7 @@
         <v>4.95E-06</v>
       </c>
       <c r="H5">
-        <v>0.004</v>
+        <v>5.59E-05</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -4024,7 +4024,7 @@
         <v>1.06E-07</v>
       </c>
       <c r="H6">
-        <v>3.81E-05</v>
+        <v>5.33E-07</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -4050,7 +4050,7 @@
         <v>4.36E-05</v>
       </c>
       <c r="H7">
-        <v>0.0143</v>
+        <v>0.000199</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -4076,7 +4076,7 @@
         <v>0.000233</v>
       </c>
       <c r="H8">
-        <v>0.00554</v>
+        <v>7.75E-05</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -4102,7 +4102,7 @@
         <v>1.82E-06</v>
       </c>
       <c r="H9">
-        <v>8.11E-06</v>
+        <v>1.13E-07</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -4128,7 +4128,7 @@
         <v>4.47E-13</v>
       </c>
       <c r="H10">
-        <v>4.85E-11</v>
+        <v>6.79E-13</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -4154,7 +4154,7 @@
         <v>1.79E-10</v>
       </c>
       <c r="H11">
-        <v>1.22E-09</v>
+        <v>1.7E-11</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -4180,7 +4180,7 @@
         <v>1.68E-13</v>
       </c>
       <c r="H12">
-        <v>1.01E-10</v>
+        <v>1.42E-12</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -4206,7 +4206,7 @@
         <v>2.27E-08</v>
       </c>
       <c r="H13">
-        <v>2.22E-05</v>
+        <v>3.11E-07</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -4232,7 +4232,7 @@
         <v>1.54E-06</v>
       </c>
       <c r="H14">
-        <v>0.000427</v>
+        <v>5.97E-06</v>
       </c>
     </row>
   </sheetData>
@@ -4316,7 +4316,7 @@
         <v>1.54E-07</v>
       </c>
       <c r="H4">
-        <v>7.37E-05</v>
+        <v>1.03E-06</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -4342,7 +4342,7 @@
         <v>5.05E-06</v>
       </c>
       <c r="H5">
-        <v>0.004</v>
+        <v>5.59E-05</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -4368,7 +4368,7 @@
         <v>1.08E-07</v>
       </c>
       <c r="H6">
-        <v>3.81E-05</v>
+        <v>5.33E-07</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -4394,7 +4394,7 @@
         <v>4.45E-05</v>
       </c>
       <c r="H7">
-        <v>0.0143</v>
+        <v>0.000199</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -4420,7 +4420,7 @@
         <v>0.000238</v>
       </c>
       <c r="H8">
-        <v>0.00554</v>
+        <v>7.75E-05</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -4446,7 +4446,7 @@
         <v>1.86E-06</v>
       </c>
       <c r="H9">
-        <v>8.11E-06</v>
+        <v>1.13E-07</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -4472,7 +4472,7 @@
         <v>4.56E-13</v>
       </c>
       <c r="H10">
-        <v>4.85E-11</v>
+        <v>6.79E-13</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -4498,7 +4498,7 @@
         <v>1.83E-10</v>
       </c>
       <c r="H11">
-        <v>1.22E-09</v>
+        <v>1.7E-11</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -4524,7 +4524,7 @@
         <v>1.71E-13</v>
       </c>
       <c r="H12">
-        <v>1.01E-10</v>
+        <v>1.42E-12</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -4550,7 +4550,7 @@
         <v>2.32E-08</v>
       </c>
       <c r="H13">
-        <v>2.22E-05</v>
+        <v>3.11E-07</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -4576,7 +4576,7 @@
         <v>1.57E-06</v>
       </c>
       <c r="H14">
-        <v>0.000427</v>
+        <v>5.97E-06</v>
       </c>
     </row>
   </sheetData>
@@ -4660,7 +4660,7 @@
         <v>1.65E-07</v>
       </c>
       <c r="H4">
-        <v>7.37E-05</v>
+        <v>1.03E-06</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -4686,7 +4686,7 @@
         <v>5.4E-06</v>
       </c>
       <c r="H5">
-        <v>0.004</v>
+        <v>5.59E-05</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -4712,7 +4712,7 @@
         <v>1.15E-07</v>
       </c>
       <c r="H6">
-        <v>3.81E-05</v>
+        <v>5.33E-07</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -4738,7 +4738,7 @@
         <v>4.76E-05</v>
       </c>
       <c r="H7">
-        <v>0.0143</v>
+        <v>0.000199</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -4764,7 +4764,7 @@
         <v>0.000255</v>
       </c>
       <c r="H8">
-        <v>0.00554</v>
+        <v>7.75E-05</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -4790,7 +4790,7 @@
         <v>1.99E-06</v>
       </c>
       <c r="H9">
-        <v>8.11E-06</v>
+        <v>1.13E-07</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -4816,7 +4816,7 @@
         <v>4.88E-13</v>
       </c>
       <c r="H10">
-        <v>4.85E-11</v>
+        <v>6.79E-13</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -4842,7 +4842,7 @@
         <v>1.95E-10</v>
       </c>
       <c r="H11">
-        <v>1.22E-09</v>
+        <v>1.7E-11</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -4868,7 +4868,7 @@
         <v>1.83E-13</v>
       </c>
       <c r="H12">
-        <v>1.01E-10</v>
+        <v>1.42E-12</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -4894,7 +4894,7 @@
         <v>2.48E-08</v>
       </c>
       <c r="H13">
-        <v>2.22E-05</v>
+        <v>3.11E-07</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -4920,7 +4920,7 @@
         <v>1.68E-06</v>
       </c>
       <c r="H14">
-        <v>0.000427</v>
+        <v>5.97E-06</v>
       </c>
     </row>
   </sheetData>
@@ -5004,7 +5004,7 @@
         <v>1.54E-07</v>
       </c>
       <c r="H4">
-        <v>7.37E-05</v>
+        <v>1.03E-06</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -5030,7 +5030,7 @@
         <v>5.04E-06</v>
       </c>
       <c r="H5">
-        <v>0.004</v>
+        <v>5.59E-05</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -5056,7 +5056,7 @@
         <v>1.08E-07</v>
       </c>
       <c r="H6">
-        <v>3.81E-05</v>
+        <v>5.33E-07</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -5082,7 +5082,7 @@
         <v>4.44E-05</v>
       </c>
       <c r="H7">
-        <v>0.0143</v>
+        <v>0.000199</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -5108,7 +5108,7 @@
         <v>0.000237</v>
       </c>
       <c r="H8">
-        <v>0.00554</v>
+        <v>7.75E-05</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -5134,7 +5134,7 @@
         <v>1.86E-06</v>
       </c>
       <c r="H9">
-        <v>8.11E-06</v>
+        <v>1.13E-07</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -5160,7 +5160,7 @@
         <v>4.55E-13</v>
       </c>
       <c r="H10">
-        <v>4.85E-11</v>
+        <v>6.79E-13</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -5186,7 +5186,7 @@
         <v>1.82E-10</v>
       </c>
       <c r="H11">
-        <v>1.22E-09</v>
+        <v>1.7E-11</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -5212,7 +5212,7 @@
         <v>1.71E-13</v>
       </c>
       <c r="H12">
-        <v>1.01E-10</v>
+        <v>1.42E-12</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -5238,7 +5238,7 @@
         <v>2.31E-08</v>
       </c>
       <c r="H13">
-        <v>2.22E-05</v>
+        <v>3.11E-07</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -5264,7 +5264,7 @@
         <v>1.57E-06</v>
       </c>
       <c r="H14">
-        <v>0.000427</v>
+        <v>5.97E-06</v>
       </c>
     </row>
   </sheetData>
@@ -5348,7 +5348,7 @@
         <v>1.46E-07</v>
       </c>
       <c r="H4">
-        <v>7.37E-05</v>
+        <v>1.03E-06</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -5374,7 +5374,7 @@
         <v>4.78E-06</v>
       </c>
       <c r="H5">
-        <v>0.004</v>
+        <v>5.59E-05</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -5400,7 +5400,7 @@
         <v>1.02E-07</v>
       </c>
       <c r="H6">
-        <v>3.81E-05</v>
+        <v>5.33E-07</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -5426,7 +5426,7 @@
         <v>4.22E-05</v>
       </c>
       <c r="H7">
-        <v>0.0143</v>
+        <v>0.000199</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -5452,7 +5452,7 @@
         <v>0.000226</v>
       </c>
       <c r="H8">
-        <v>0.00554</v>
+        <v>7.75E-05</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -5478,7 +5478,7 @@
         <v>1.76E-06</v>
       </c>
       <c r="H9">
-        <v>8.11E-06</v>
+        <v>1.13E-07</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -5504,7 +5504,7 @@
         <v>4.32E-13</v>
       </c>
       <c r="H10">
-        <v>4.85E-11</v>
+        <v>6.79E-13</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -5530,7 +5530,7 @@
         <v>1.73E-10</v>
       </c>
       <c r="H11">
-        <v>1.22E-09</v>
+        <v>1.7E-11</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -5556,7 +5556,7 @@
         <v>1.62E-13</v>
       </c>
       <c r="H12">
-        <v>1.01E-10</v>
+        <v>1.42E-12</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -5582,7 +5582,7 @@
         <v>2.2E-08</v>
       </c>
       <c r="H13">
-        <v>2.22E-05</v>
+        <v>3.11E-07</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -5608,7 +5608,7 @@
         <v>1.49E-06</v>
       </c>
       <c r="H14">
-        <v>0.000427</v>
+        <v>5.97E-06</v>
       </c>
     </row>
   </sheetData>
@@ -5692,7 +5692,7 @@
         <v>2.83E-08</v>
       </c>
       <c r="H4">
-        <v>7.37E-05</v>
+        <v>1.03E-06</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -5718,7 +5718,7 @@
         <v>9.29E-07</v>
       </c>
       <c r="H5">
-        <v>0.004</v>
+        <v>5.59E-05</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -5744,7 +5744,7 @@
         <v>1.98E-08</v>
       </c>
       <c r="H6">
-        <v>3.81E-05</v>
+        <v>5.33E-07</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -5770,7 +5770,7 @@
         <v>8.199999999999999E-06</v>
       </c>
       <c r="H7">
-        <v>0.0143</v>
+        <v>0.000199</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -5796,7 +5796,7 @@
         <v>4.38E-05</v>
       </c>
       <c r="H8">
-        <v>0.00554</v>
+        <v>7.75E-05</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -5822,7 +5822,7 @@
         <v>3.42E-07</v>
       </c>
       <c r="H9">
-        <v>8.11E-06</v>
+        <v>1.13E-07</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -5848,7 +5848,7 @@
         <v>8.4E-14</v>
       </c>
       <c r="H10">
-        <v>4.85E-11</v>
+        <v>6.79E-13</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -5874,7 +5874,7 @@
         <v>3.36E-11</v>
       </c>
       <c r="H11">
-        <v>1.22E-09</v>
+        <v>1.7E-11</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -5900,7 +5900,7 @@
         <v>3.15E-14</v>
       </c>
       <c r="H12">
-        <v>1.01E-10</v>
+        <v>1.42E-12</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -5926,7 +5926,7 @@
         <v>4.26E-09</v>
       </c>
       <c r="H13">
-        <v>2.22E-05</v>
+        <v>3.11E-07</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -5952,7 +5952,7 @@
         <v>2.9E-07</v>
       </c>
       <c r="H14">
-        <v>0.000427</v>
+        <v>5.97E-06</v>
       </c>
     </row>
   </sheetData>
@@ -6036,7 +6036,7 @@
         <v>2.15E-08</v>
       </c>
       <c r="H4">
-        <v>7.37E-05</v>
+        <v>1.03E-06</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -6062,7 +6062,7 @@
         <v>7.06E-07</v>
       </c>
       <c r="H5">
-        <v>0.004</v>
+        <v>5.59E-05</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -6088,7 +6088,7 @@
         <v>1.51E-08</v>
       </c>
       <c r="H6">
-        <v>3.81E-05</v>
+        <v>5.33E-07</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -6114,7 +6114,7 @@
         <v>6.23E-06</v>
       </c>
       <c r="H7">
-        <v>0.0143</v>
+        <v>0.000199</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -6140,7 +6140,7 @@
         <v>3.33E-05</v>
       </c>
       <c r="H8">
-        <v>0.00554</v>
+        <v>7.75E-05</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -6166,7 +6166,7 @@
         <v>2.6E-07</v>
       </c>
       <c r="H9">
-        <v>8.11E-06</v>
+        <v>1.13E-07</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -6192,7 +6192,7 @@
         <v>6.38E-14</v>
       </c>
       <c r="H10">
-        <v>4.85E-11</v>
+        <v>6.79E-13</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -6218,7 +6218,7 @@
         <v>2.55E-11</v>
       </c>
       <c r="H11">
-        <v>1.22E-09</v>
+        <v>1.7E-11</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -6244,7 +6244,7 @@
         <v>2.39E-14</v>
       </c>
       <c r="H12">
-        <v>1.01E-10</v>
+        <v>1.42E-12</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -6270,7 +6270,7 @@
         <v>3.24E-09</v>
       </c>
       <c r="H13">
-        <v>2.22E-05</v>
+        <v>3.11E-07</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -6296,7 +6296,7 @@
         <v>2.2E-07</v>
       </c>
       <c r="H14">
-        <v>0.000427</v>
+        <v>5.97E-06</v>
       </c>
     </row>
   </sheetData>
@@ -6380,7 +6380,7 @@
         <v>2.26E-08</v>
       </c>
       <c r="H4">
-        <v>7.37E-05</v>
+        <v>1.03E-06</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -6406,7 +6406,7 @@
         <v>7.43E-07</v>
       </c>
       <c r="H5">
-        <v>0.004</v>
+        <v>5.59E-05</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -6432,7 +6432,7 @@
         <v>1.59E-08</v>
       </c>
       <c r="H6">
-        <v>3.81E-05</v>
+        <v>5.33E-07</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -6458,7 +6458,7 @@
         <v>6.55E-06</v>
       </c>
       <c r="H7">
-        <v>0.0143</v>
+        <v>0.000199</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -6484,7 +6484,7 @@
         <v>3.5E-05</v>
       </c>
       <c r="H8">
-        <v>0.00554</v>
+        <v>7.75E-05</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -6510,7 +6510,7 @@
         <v>2.74E-07</v>
       </c>
       <c r="H9">
-        <v>8.11E-06</v>
+        <v>1.13E-07</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -6536,7 +6536,7 @@
         <v>6.71E-14</v>
       </c>
       <c r="H10">
-        <v>4.85E-11</v>
+        <v>6.79E-13</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -6562,7 +6562,7 @@
         <v>2.69E-11</v>
       </c>
       <c r="H11">
-        <v>1.22E-09</v>
+        <v>1.7E-11</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -6588,7 +6588,7 @@
         <v>2.52E-14</v>
       </c>
       <c r="H12">
-        <v>1.01E-10</v>
+        <v>1.42E-12</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -6614,7 +6614,7 @@
         <v>3.41E-09</v>
       </c>
       <c r="H13">
-        <v>2.22E-05</v>
+        <v>3.11E-07</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -6640,7 +6640,7 @@
         <v>2.31E-07</v>
       </c>
       <c r="H14">
-        <v>0.000427</v>
+        <v>5.97E-06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>